<commit_message>
Added OtherStudentsComments Performance test; Report on first load test scenario for ExamRegistering;
</commit_message>
<xml_diff>
--- a/ReportsOnArcherWebAndLoadTests/WebPerformanceReports_draft1.xlsx
+++ b/ReportsOnArcherWebAndLoadTests/WebPerformanceReports_draft1.xlsx
@@ -5,14 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\003. SQA\LoadExercises\ArcherWebAndLoadTestProject1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QATeamArcher\ReportsOnArcherWebAndLoadTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Homework" sheetId="3" r:id="rId1"/>
+    <sheet name="ExamRegistering1" sheetId="5" r:id="rId2"/>
+    <sheet name="ExamRegistering2" sheetId="6" r:id="rId3"/>
+    <sheet name="Other Students Comments" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="252">
   <si>
     <t>Passed</t>
   </si>
@@ -258,6 +261,528 @@
   </si>
   <si>
     <t>Response Bytes</t>
+  </si>
+  <si>
+    <t>7.443 sec</t>
+  </si>
+  <si>
+    <t>0.547 sec</t>
+  </si>
+  <si>
+    <t>3.307 sec</t>
+  </si>
+  <si>
+    <t>2.047 sec</t>
+  </si>
+  <si>
+    <t>0.172 sec</t>
+  </si>
+  <si>
+    <t>3.442 sec</t>
+  </si>
+  <si>
+    <t>0.401 sec</t>
+  </si>
+  <si>
+    <t>3.909 sec</t>
+  </si>
+  <si>
+    <t>http://stage.telerikacademy.com/Courses/HomeworkEvaluations/ViewMyEvaluations/55</t>
+  </si>
+  <si>
+    <t>3.112 sec</t>
+  </si>
+  <si>
+    <t>4.181 sec</t>
+  </si>
+  <si>
+    <t>0.228 sec</t>
+  </si>
+  <si>
+    <t>0.215 sec</t>
+  </si>
+  <si>
+    <t>4.736 sec</t>
+  </si>
+  <si>
+    <t>0.575 sec</t>
+  </si>
+  <si>
+    <t>3.122 sec</t>
+  </si>
+  <si>
+    <t>0.207 sec</t>
+  </si>
+  <si>
+    <t>2.262 sec</t>
+  </si>
+  <si>
+    <t>0.181 sec</t>
+  </si>
+  <si>
+    <t>3.662 sec</t>
+  </si>
+  <si>
+    <t>0.404 sec</t>
+  </si>
+  <si>
+    <t>0.220 sec</t>
+  </si>
+  <si>
+    <t>2.357 sec</t>
+  </si>
+  <si>
+    <t>0.202 sec</t>
+  </si>
+  <si>
+    <t>4.313 sec</t>
+  </si>
+  <si>
+    <t>0.216 sec</t>
+  </si>
+  <si>
+    <t>5.393 sec</t>
+  </si>
+  <si>
+    <t>0.227 sec</t>
+  </si>
+  <si>
+    <t>3.366 sec</t>
+  </si>
+  <si>
+    <t>0.608 sec</t>
+  </si>
+  <si>
+    <t>2.036 sec</t>
+  </si>
+  <si>
+    <t>0.175 sec</t>
+  </si>
+  <si>
+    <t>2.666 sec</t>
+  </si>
+  <si>
+    <t>0.085 sec</t>
+  </si>
+  <si>
+    <t>3.517 sec</t>
+  </si>
+  <si>
+    <t>0.408 sec</t>
+  </si>
+  <si>
+    <t>0.235 sec</t>
+  </si>
+  <si>
+    <t>2.292 sec</t>
+  </si>
+  <si>
+    <t>0.238 sec</t>
+  </si>
+  <si>
+    <t>2.711 sec</t>
+  </si>
+  <si>
+    <t>0.242 sec</t>
+  </si>
+  <si>
+    <t>4.334 sec</t>
+  </si>
+  <si>
+    <t>7.693 sec</t>
+  </si>
+  <si>
+    <t>2.790 sec</t>
+  </si>
+  <si>
+    <t>3.890 sec</t>
+  </si>
+  <si>
+    <t>0.166 sec</t>
+  </si>
+  <si>
+    <t>4.300 sec</t>
+  </si>
+  <si>
+    <t>0.380 sec</t>
+  </si>
+  <si>
+    <t>0.199 sec</t>
+  </si>
+  <si>
+    <t>http://stage.telerikacademy.com/Courses/PracticalExams/Select/265</t>
+  </si>
+  <si>
+    <t>4.759 sec</t>
+  </si>
+  <si>
+    <t>5.376 sec</t>
+  </si>
+  <si>
+    <t>3.728 sec</t>
+  </si>
+  <si>
+    <t>0.206 sec</t>
+  </si>
+  <si>
+    <t>3.109 sec</t>
+  </si>
+  <si>
+    <t>0.222 sec</t>
+  </si>
+  <si>
+    <t>4.525 sec</t>
+  </si>
+  <si>
+    <t>3.294 sec</t>
+  </si>
+  <si>
+    <t>0.190 sec</t>
+  </si>
+  <si>
+    <t>4.528 sec</t>
+  </si>
+  <si>
+    <t>0.198 sec</t>
+  </si>
+  <si>
+    <t>5.131 sec</t>
+  </si>
+  <si>
+    <t>0.192 sec</t>
+  </si>
+  <si>
+    <t>5.532 sec</t>
+  </si>
+  <si>
+    <t>5.795 sec</t>
+  </si>
+  <si>
+    <t>0.191 sec</t>
+  </si>
+  <si>
+    <t>3.313 sec</t>
+  </si>
+  <si>
+    <t>0.587 sec</t>
+  </si>
+  <si>
+    <t>2.463 sec</t>
+  </si>
+  <si>
+    <t>0.183 sec</t>
+  </si>
+  <si>
+    <t>3.696 sec</t>
+  </si>
+  <si>
+    <t>0.392 sec</t>
+  </si>
+  <si>
+    <t>0.226 sec</t>
+  </si>
+  <si>
+    <t>3.925 sec</t>
+  </si>
+  <si>
+    <t>0.200 sec</t>
+  </si>
+  <si>
+    <t>3.298 sec</t>
+  </si>
+  <si>
+    <t>4.351 sec</t>
+  </si>
+  <si>
+    <t>5.763 sec</t>
+  </si>
+  <si>
+    <t>0.196 sec</t>
+  </si>
+  <si>
+    <t>5.778 sec</t>
+  </si>
+  <si>
+    <t>0.218 sec</t>
+  </si>
+  <si>
+    <t>5.541 sec</t>
+  </si>
+  <si>
+    <t>0.195 sec</t>
+  </si>
+  <si>
+    <t>5.762 sec</t>
+  </si>
+  <si>
+    <t>5.138 sec</t>
+  </si>
+  <si>
+    <t>0.064 sec</t>
+  </si>
+  <si>
+    <t>5.336 sec</t>
+  </si>
+  <si>
+    <t>5.749 sec</t>
+  </si>
+  <si>
+    <t>5.777 sec</t>
+  </si>
+  <si>
+    <t>0.189 sec</t>
+  </si>
+  <si>
+    <t>5.443 sec</t>
+  </si>
+  <si>
+    <t>0.597 sec</t>
+  </si>
+  <si>
+    <t>3.394 sec</t>
+  </si>
+  <si>
+    <t>0.097 sec</t>
+  </si>
+  <si>
+    <t>4.089 sec</t>
+  </si>
+  <si>
+    <t>0.383 sec</t>
+  </si>
+  <si>
+    <t>0.217 sec</t>
+  </si>
+  <si>
+    <t>3.300 sec</t>
+  </si>
+  <si>
+    <t>4.883 sec</t>
+  </si>
+  <si>
+    <t>3.584 sec</t>
+  </si>
+  <si>
+    <t>0.091 sec</t>
+  </si>
+  <si>
+    <t>5.167 sec</t>
+  </si>
+  <si>
+    <t>3.753 sec</t>
+  </si>
+  <si>
+    <t>7.971 sec</t>
+  </si>
+  <si>
+    <t>0.179 sec</t>
+  </si>
+  <si>
+    <t>6.383 sec</t>
+  </si>
+  <si>
+    <t>0.193 sec</t>
+  </si>
+  <si>
+    <t>6.440 sec</t>
+  </si>
+  <si>
+    <t>6.565 sec</t>
+  </si>
+  <si>
+    <t>0.176 sec</t>
+  </si>
+  <si>
+    <t>6.360 sec</t>
+  </si>
+  <si>
+    <t>6.194 sec</t>
+  </si>
+  <si>
+    <t>7.380 sec</t>
+  </si>
+  <si>
+    <t>2.466 sec</t>
+  </si>
+  <si>
+    <t>4.445 sec</t>
+  </si>
+  <si>
+    <t>5.746 sec</t>
+  </si>
+  <si>
+    <t>0.182 sec</t>
+  </si>
+  <si>
+    <t>7.271 sec</t>
+  </si>
+  <si>
+    <t>6.680 sec</t>
+  </si>
+  <si>
+    <t>0.048 sec</t>
+  </si>
+  <si>
+    <t>6.595 sec</t>
+  </si>
+  <si>
+    <t>6.144 sec</t>
+  </si>
+  <si>
+    <t>6.621 sec</t>
+  </si>
+  <si>
+    <t>6.612 sec</t>
+  </si>
+  <si>
+    <t>6.641 sec</t>
+  </si>
+  <si>
+    <t>0.051 sec</t>
+  </si>
+  <si>
+    <t>3.895 sec</t>
+  </si>
+  <si>
+    <t>0.187 sec</t>
+  </si>
+  <si>
+    <t>5.587 sec</t>
+  </si>
+  <si>
+    <t>0.050 sec</t>
+  </si>
+  <si>
+    <t>6.754 sec</t>
+  </si>
+  <si>
+    <t>4.324 sec</t>
+  </si>
+  <si>
+    <t>0.610 sec</t>
+  </si>
+  <si>
+    <t>3.508 sec</t>
+  </si>
+  <si>
+    <t>0.021 sec</t>
+  </si>
+  <si>
+    <t>3.093 sec</t>
+  </si>
+  <si>
+    <t>0.029 sec</t>
+  </si>
+  <si>
+    <t>0.100 sec</t>
+  </si>
+  <si>
+    <t>2.748 sec</t>
+  </si>
+  <si>
+    <t>2.709 sec</t>
+  </si>
+  <si>
+    <t>4.122 sec</t>
+  </si>
+  <si>
+    <t>0.177 sec</t>
+  </si>
+  <si>
+    <t>3.290 sec</t>
+  </si>
+  <si>
+    <t>3.110 sec</t>
+  </si>
+  <si>
+    <t>3.894 sec</t>
+  </si>
+  <si>
+    <t>3.494 sec</t>
+  </si>
+  <si>
+    <t>0.186 sec</t>
+  </si>
+  <si>
+    <t>3.091 sec</t>
+  </si>
+  <si>
+    <t>0.046 sec</t>
+  </si>
+  <si>
+    <t>4.892 sec</t>
+  </si>
+  <si>
+    <t>0.184 sec</t>
+  </si>
+  <si>
+    <t>4.549 sec</t>
+  </si>
+  <si>
+    <t>4.939 sec</t>
+  </si>
+  <si>
+    <t>4.544 sec</t>
+  </si>
+  <si>
+    <t>0.602 sec</t>
+  </si>
+  <si>
+    <t>4.575 sec</t>
+  </si>
+  <si>
+    <t>0.024 sec</t>
+  </si>
+  <si>
+    <t>4.960 sec</t>
+  </si>
+  <si>
+    <t>5.181 sec</t>
+  </si>
+  <si>
+    <t>0.038 sec</t>
+  </si>
+  <si>
+    <t>5.392 sec</t>
+  </si>
+  <si>
+    <t>0.240 sec</t>
+  </si>
+  <si>
+    <t>5.349 sec</t>
+  </si>
+  <si>
+    <t>0.047 sec</t>
+  </si>
+  <si>
+    <t>7.214 sec</t>
+  </si>
+  <si>
+    <t>5.134 sec</t>
+  </si>
+  <si>
+    <t>0.197 sec</t>
+  </si>
+  <si>
+    <t>5.526 sec</t>
+  </si>
+  <si>
+    <t>4.383 sec</t>
+  </si>
+  <si>
+    <t>0.049 sec</t>
+  </si>
+  <si>
+    <t>5.326 sec</t>
+  </si>
+  <si>
+    <t>0.170 sec</t>
+  </si>
+  <si>
+    <t>5.399 sec</t>
+  </si>
+  <si>
+    <t>6.202 sec</t>
   </si>
 </sst>
 </file>
@@ -578,7 +1103,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1325,4 +1852,2604 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="64" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3291111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3375513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" t="s">
+        <v>138</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" t="s">
+        <v>140</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" t="s">
+        <v>143</v>
+      </c>
+      <c r="F16">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>144</v>
+      </c>
+      <c r="E20" t="s">
+        <v>145</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3291111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F22">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F23" s="1">
+        <v>3375513</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>151</v>
+      </c>
+      <c r="E24" t="s">
+        <v>152</v>
+      </c>
+      <c r="F24" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26" t="s">
+        <v>152</v>
+      </c>
+      <c r="F26" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E27" t="s">
+        <v>156</v>
+      </c>
+      <c r="F27" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>157</v>
+      </c>
+      <c r="E28" t="s">
+        <v>158</v>
+      </c>
+      <c r="F28" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>159</v>
+      </c>
+      <c r="E29" t="s">
+        <v>160</v>
+      </c>
+      <c r="F29" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>161</v>
+      </c>
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>162</v>
+      </c>
+      <c r="E31" t="s">
+        <v>163</v>
+      </c>
+      <c r="F31" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>164</v>
+      </c>
+      <c r="E32" t="s">
+        <v>160</v>
+      </c>
+      <c r="F32" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>165</v>
+      </c>
+      <c r="E33" t="s">
+        <v>156</v>
+      </c>
+      <c r="F33" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" t="s">
+        <v>166</v>
+      </c>
+      <c r="E34" t="s">
+        <v>167</v>
+      </c>
+      <c r="F34">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>168</v>
+      </c>
+      <c r="E38" t="s">
+        <v>169</v>
+      </c>
+      <c r="F38" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>170</v>
+      </c>
+      <c r="E39" t="s">
+        <v>171</v>
+      </c>
+      <c r="F39" s="1">
+        <v>3291111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E40" t="s">
+        <v>173</v>
+      </c>
+      <c r="F40">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F41" s="1">
+        <v>3375513</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>127</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>175</v>
+      </c>
+      <c r="E42" t="s">
+        <v>174</v>
+      </c>
+      <c r="F42" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>176</v>
+      </c>
+      <c r="E43" t="s">
+        <v>30</v>
+      </c>
+      <c r="F43" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>177</v>
+      </c>
+      <c r="E44" t="s">
+        <v>178</v>
+      </c>
+      <c r="F44" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>179</v>
+      </c>
+      <c r="E45" t="s">
+        <v>133</v>
+      </c>
+      <c r="F45" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>180</v>
+      </c>
+      <c r="E46" t="s">
+        <v>158</v>
+      </c>
+      <c r="F46" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s">
+        <v>181</v>
+      </c>
+      <c r="E47" t="s">
+        <v>182</v>
+      </c>
+      <c r="F47" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>183</v>
+      </c>
+      <c r="E48" t="s">
+        <v>184</v>
+      </c>
+      <c r="F48" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>127</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>185</v>
+      </c>
+      <c r="E49" t="s">
+        <v>184</v>
+      </c>
+      <c r="F49" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>186</v>
+      </c>
+      <c r="E50" t="s">
+        <v>187</v>
+      </c>
+      <c r="F50" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>188</v>
+      </c>
+      <c r="E51" t="s">
+        <v>160</v>
+      </c>
+      <c r="F51" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" t="s">
+        <v>189</v>
+      </c>
+      <c r="E52" t="s">
+        <v>140</v>
+      </c>
+      <c r="F52">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F53" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="64" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3373993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3291111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F5">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3376117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3376117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3376117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>200</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3376117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E13" t="s">
+        <v>160</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>202</v>
+      </c>
+      <c r="E14" t="s">
+        <v>203</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3376117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>204</v>
+      </c>
+      <c r="E15" t="s">
+        <v>205</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>206</v>
+      </c>
+      <c r="E16" t="s">
+        <v>207</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3376117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>208</v>
+      </c>
+      <c r="E17" t="s">
+        <v>143</v>
+      </c>
+      <c r="F17">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>209</v>
+      </c>
+      <c r="E21" t="s">
+        <v>210</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>211</v>
+      </c>
+      <c r="E22" t="s">
+        <v>212</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3291111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>213</v>
+      </c>
+      <c r="E23" t="s">
+        <v>214</v>
+      </c>
+      <c r="F23">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>215</v>
+      </c>
+      <c r="F24" s="1">
+        <v>3375513</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E25" t="s">
+        <v>197</v>
+      </c>
+      <c r="F25" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>217</v>
+      </c>
+      <c r="E26" t="s">
+        <v>131</v>
+      </c>
+      <c r="F26" s="1">
+        <v>3375513</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>218</v>
+      </c>
+      <c r="E27" t="s">
+        <v>219</v>
+      </c>
+      <c r="F27" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>220</v>
+      </c>
+      <c r="E28" t="s">
+        <v>197</v>
+      </c>
+      <c r="F28" s="1">
+        <v>3375513</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>221</v>
+      </c>
+      <c r="E29" t="s">
+        <v>167</v>
+      </c>
+      <c r="F29" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>222</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="1">
+        <v>3375513</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>223</v>
+      </c>
+      <c r="E31" t="s">
+        <v>224</v>
+      </c>
+      <c r="F31" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>225</v>
+      </c>
+      <c r="E32" t="s">
+        <v>226</v>
+      </c>
+      <c r="F32" s="1">
+        <v>3375513</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>227</v>
+      </c>
+      <c r="E33" t="s">
+        <v>228</v>
+      </c>
+      <c r="F33" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>229</v>
+      </c>
+      <c r="E34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" s="1">
+        <v>3375513</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" t="s">
+        <v>230</v>
+      </c>
+      <c r="E35" t="s">
+        <v>228</v>
+      </c>
+      <c r="F35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>174</v>
+      </c>
+      <c r="F36" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>231</v>
+      </c>
+      <c r="E39" t="s">
+        <v>232</v>
+      </c>
+      <c r="F39" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>233</v>
+      </c>
+      <c r="E40" t="s">
+        <v>234</v>
+      </c>
+      <c r="F40" s="1">
+        <v>3291111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" t="s">
+        <v>235</v>
+      </c>
+      <c r="E41" t="s">
+        <v>105</v>
+      </c>
+      <c r="F41">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>94</v>
+      </c>
+      <c r="F42" s="1">
+        <v>3375513</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>236</v>
+      </c>
+      <c r="E43" t="s">
+        <v>237</v>
+      </c>
+      <c r="F43" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>238</v>
+      </c>
+      <c r="E44" t="s">
+        <v>239</v>
+      </c>
+      <c r="F44" s="1">
+        <v>3375513</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>240</v>
+      </c>
+      <c r="E45" t="s">
+        <v>156</v>
+      </c>
+      <c r="F45" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>240</v>
+      </c>
+      <c r="E46" t="s">
+        <v>241</v>
+      </c>
+      <c r="F46" s="1">
+        <v>3375513</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s">
+        <v>242</v>
+      </c>
+      <c r="E47" t="s">
+        <v>94</v>
+      </c>
+      <c r="F47" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>243</v>
+      </c>
+      <c r="E48" t="s">
+        <v>244</v>
+      </c>
+      <c r="F48" s="1">
+        <v>3375513</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>127</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>245</v>
+      </c>
+      <c r="E49" t="s">
+        <v>205</v>
+      </c>
+      <c r="F49" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>246</v>
+      </c>
+      <c r="E50" t="s">
+        <v>247</v>
+      </c>
+      <c r="F50" s="1">
+        <v>3375513</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>248</v>
+      </c>
+      <c r="E51" t="s">
+        <v>249</v>
+      </c>
+      <c r="F51" s="1">
+        <v>3282766</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>250</v>
+      </c>
+      <c r="E52" t="s">
+        <v>226</v>
+      </c>
+      <c r="F52" s="1">
+        <v>3375513</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" t="s">
+        <v>251</v>
+      </c>
+      <c r="E53" t="s">
+        <v>33</v>
+      </c>
+      <c r="F53">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3291111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3375421</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3288737</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3282251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3291111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3375421</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3288742</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" t="s">
+        <v>103</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3282251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" t="s">
+        <v>107</v>
+      </c>
+      <c r="F25" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" s="1">
+        <v>3291111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="1">
+        <v>3375421</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="1">
+        <v>3288738</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" t="s">
+        <v>118</v>
+      </c>
+      <c r="F31" s="1">
+        <v>3282251</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" t="s">
+        <v>119</v>
+      </c>
+      <c r="E32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>90</v>
+      </c>
+      <c r="F33" s="1">
+        <v>3373085</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>